<commit_message>
Updating Images Folder, ppt & accuracy report
</commit_message>
<xml_diff>
--- a/Presentation & reports/Accuracy Report.xlsx
+++ b/Presentation & reports/Accuracy Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praga\Desktop\SheLLLearn WIP\Presentation &amp; reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praga\OneDrive\Documents\Rutgers\Rutgers_Assignments&amp;Projects\Learn2Write\Presentation &amp; reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EABAE27-87D7-41BB-8BE1-CE14169A168F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3ABB99-F72C-4E37-96BF-36545FB40BF6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1B2B95F-E12E-4163-ADBF-CCFD1D4B5382}"/>
   </bookViews>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B10DA0-767C-4167-9BBE-469C2D35444B}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>